<commit_message>
terminal o/p del keyfile
</commit_message>
<xml_diff>
--- a/bank_records.xlsx
+++ b/bank_records.xlsx
@@ -523,7 +523,7 @@
         <v>223</v>
       </c>
       <c r="C6" t="n">
-        <v>906</v>
+        <v>881</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>46007</v>
@@ -551,7 +551,7 @@
         <v>112</v>
       </c>
       <c r="C8" t="n">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>46009</v>

</xml_diff>

<commit_message>
time and memory measured
</commit_message>
<xml_diff>
--- a/bank_records.xlsx
+++ b/bank_records.xlsx
@@ -523,7 +523,7 @@
         <v>223</v>
       </c>
       <c r="C6" t="n">
-        <v>881</v>
+        <v>891</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>46007</v>
@@ -551,7 +551,7 @@
         <v>112</v>
       </c>
       <c r="C8" t="n">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>46009</v>

</xml_diff>